<commit_message>
updated order on search
</commit_message>
<xml_diff>
--- a/markdown/scripts/DawnChorus.xlsx
+++ b/markdown/scripts/DawnChorus.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="DawnChorus.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -55,12 +55,18 @@
     <t>Eastern whip-poor-will</t>
   </si>
   <si>
+    <t>VA-37</t>
+  </si>
+  <si>
     <t>Nightjars</t>
   </si>
   <si>
     <t>Least flycatcher</t>
   </si>
   <si>
+    <t>VA-55</t>
+  </si>
+  <si>
     <t xml:space="preserve">Flycatchers </t>
   </si>
   <si>
@@ -70,24 +76,39 @@
     <t>Great crested flycatcher</t>
   </si>
   <si>
+    <t>VA-27</t>
+  </si>
+  <si>
     <t>Eastern kingbird</t>
   </si>
   <si>
+    <t>VA-85</t>
+  </si>
+  <si>
     <t>Blue-gray gnatcatcher</t>
   </si>
   <si>
+    <t>VA-24</t>
+  </si>
+  <si>
     <t>Gnatcatchers, kinglets, wrentit</t>
   </si>
   <si>
     <t>American robin</t>
   </si>
   <si>
+    <t>VA-53</t>
+  </si>
+  <si>
     <t>Thrushes</t>
   </si>
   <si>
     <t>Brown thrasher</t>
   </si>
   <si>
+    <t>VA-30</t>
+  </si>
+  <si>
     <t>Mockingbirds, catbirds, thrashers</t>
   </si>
   <si>
@@ -97,69 +118,126 @@
     <t>Blue-winged warbler</t>
   </si>
   <si>
+    <t>VA-73</t>
+  </si>
+  <si>
     <t>Warblers</t>
   </si>
   <si>
     <t>Black-and-white warbler</t>
   </si>
   <si>
+    <t>VA-74</t>
+  </si>
+  <si>
     <t>Common yellowthroat</t>
   </si>
   <si>
+    <t>VA-22</t>
+  </si>
+  <si>
     <t>Hooded warbler</t>
   </si>
   <si>
+    <t>VA-76</t>
+  </si>
+  <si>
     <t>Chestnut-sided warbler</t>
   </si>
   <si>
+    <t>VA-43</t>
+  </si>
+  <si>
     <t>Black-throated green warbler</t>
   </si>
   <si>
+    <t>VA-61</t>
+  </si>
+  <si>
     <t>Canada warbler</t>
   </si>
   <si>
+    <t>VA-52</t>
+  </si>
+  <si>
     <t>Eastern towhee</t>
   </si>
   <si>
+    <t>VA-35</t>
+  </si>
+  <si>
     <t>Sparrows</t>
   </si>
   <si>
     <t>Field sparrow</t>
   </si>
   <si>
+    <t>VA-39</t>
+  </si>
+  <si>
     <t>Scarlet tanager</t>
   </si>
   <si>
+    <t>VA-38</t>
+  </si>
+  <si>
     <t>Cardinals, tanagers, grosbeaks, buntings</t>
   </si>
   <si>
     <t>Northern cardinal</t>
   </si>
   <si>
+    <t>VA-26</t>
+  </si>
+  <si>
     <t>Kentucky</t>
   </si>
   <si>
     <t>Eastern wood-pewee</t>
   </si>
   <si>
+    <t>KY-144</t>
+  </si>
+  <si>
     <t>Willow flycatcher</t>
   </si>
   <si>
+    <t>KY-82</t>
+  </si>
+  <si>
+    <t>KY-128</t>
+  </si>
+  <si>
     <t>Eastern bluebird</t>
   </si>
   <si>
+    <t>KY-72</t>
+  </si>
+  <si>
     <t>Northern mockingbird</t>
   </si>
   <si>
+    <t>KY-105</t>
+  </si>
+  <si>
     <t>American redstart</t>
   </si>
   <si>
+    <t>KY-75</t>
+  </si>
+  <si>
     <t>Yellow-breasted chat</t>
   </si>
   <si>
+    <t>KY-86</t>
+  </si>
+  <si>
     <t>House finch</t>
   </si>
   <si>
+    <t>KY-120</t>
+  </si>
+  <si>
     <t>Finches</t>
   </si>
   <si>
@@ -169,24 +247,45 @@
     <t>Illinois</t>
   </si>
   <si>
+    <t>Chuck-will's-widow</t>
+  </si>
+  <si>
+    <t>IL-127</t>
+  </si>
+  <si>
     <t>Purple martin</t>
   </si>
   <si>
+    <t>IL-126</t>
+  </si>
+  <si>
     <t>Swallows</t>
   </si>
   <si>
     <t>Larks, swallows</t>
   </si>
   <si>
+    <t>IL-88</t>
+  </si>
+  <si>
     <t>Summer tanager</t>
   </si>
   <si>
+    <t>IL-130</t>
+  </si>
+  <si>
     <t>Dickcissel</t>
   </si>
   <si>
+    <t>IL-108</t>
+  </si>
+  <si>
     <t>Orchard oriole</t>
   </si>
   <si>
+    <t>IL-146</t>
+  </si>
+  <si>
     <t>Blackbirds</t>
   </si>
   <si>
@@ -196,15 +295,30 @@
     <t>Barred owl</t>
   </si>
   <si>
+    <t>MO-13</t>
+  </si>
+  <si>
     <t>Owls</t>
   </si>
   <si>
     <t>Acadian flycatcher</t>
   </si>
   <si>
+    <t>MO-129</t>
+  </si>
+  <si>
     <t>Eastern phoebe</t>
   </si>
   <si>
+    <t>MO-150</t>
+  </si>
+  <si>
+    <t>Bell's vireo</t>
+  </si>
+  <si>
+    <t>MO-151</t>
+  </si>
+  <si>
     <t>Vireos</t>
   </si>
   <si>
@@ -214,54 +328,114 @@
     <t>Pine warbler</t>
   </si>
   <si>
+    <t>MO-140</t>
+  </si>
+  <si>
     <t>Chipping sparrow</t>
   </si>
   <si>
+    <t>MO-145</t>
+  </si>
+  <si>
     <t>Kansas</t>
   </si>
   <si>
+    <t>KS-173</t>
+  </si>
+  <si>
     <t>Western kingbird</t>
   </si>
   <si>
+    <t>KS-175</t>
+  </si>
+  <si>
+    <t>KS-174</t>
+  </si>
+  <si>
     <t>Scissor-tailed flycatcher</t>
   </si>
   <si>
+    <t>KS-176</t>
+  </si>
+  <si>
+    <t>KS-186</t>
+  </si>
+  <si>
     <t>Baltimore oriole</t>
   </si>
   <si>
+    <t>KS-177</t>
+  </si>
+  <si>
     <t>Colorado</t>
   </si>
   <si>
     <t>Gray flycatcher</t>
   </si>
   <si>
+    <t>CO-195</t>
+  </si>
+  <si>
     <t>Horned lark</t>
   </si>
   <si>
+    <t>CO-284</t>
+  </si>
+  <si>
     <t>Larks</t>
   </si>
   <si>
     <t>Hermit thrush</t>
   </si>
   <si>
+    <t>CO-256</t>
+  </si>
+  <si>
     <t>Spotted towhee</t>
   </si>
   <si>
+    <t>CO-194</t>
+  </si>
+  <si>
+    <t>Brewer's sparrow</t>
+  </si>
+  <si>
+    <t>CO-216</t>
+  </si>
+  <si>
+    <t>Lincoln's sparrow</t>
+  </si>
+  <si>
+    <t>CO-213</t>
+  </si>
+  <si>
     <t>Black-headed grosbeak</t>
   </si>
   <si>
+    <t>CO-193</t>
+  </si>
+  <si>
     <t>Yellow-headed blackbird</t>
   </si>
   <si>
+    <t>CO-280</t>
+  </si>
+  <si>
     <t>House sparrow</t>
   </si>
   <si>
+    <t>CO-139</t>
+  </si>
+  <si>
     <t>Wyoming</t>
   </si>
   <si>
     <t>Sora</t>
   </si>
   <si>
+    <t>WY-261</t>
+  </si>
+  <si>
     <t>Rails</t>
   </si>
   <si>
@@ -271,54 +445,123 @@
     <t>Mountain bluebird</t>
   </si>
   <si>
+    <t>WY-260</t>
+  </si>
+  <si>
     <t>Yellow warbler</t>
   </si>
   <si>
+    <t>WY-69</t>
+  </si>
+  <si>
     <t>Vesper sparrow</t>
   </si>
   <si>
+    <t>WY-253</t>
+  </si>
+  <si>
+    <t>Cassin's finch</t>
+  </si>
+  <si>
+    <t>WY-264</t>
+  </si>
+  <si>
     <t>Montana</t>
   </si>
   <si>
+    <t>MT-285</t>
+  </si>
+  <si>
     <t>Gray catbird</t>
   </si>
   <si>
+    <t>MT-277</t>
+  </si>
+  <si>
     <t>White-crowned sparrow</t>
   </si>
   <si>
+    <t>MT-269</t>
+  </si>
+  <si>
     <t>Idaho</t>
   </si>
   <si>
     <t>Cordilleran flycatcher</t>
   </si>
   <si>
+    <t>ID-202</t>
+  </si>
+  <si>
     <t>Veery</t>
   </si>
   <si>
+    <t>ID-323</t>
+  </si>
+  <si>
     <t>Nashville warbler</t>
   </si>
   <si>
+    <t>ID-302</t>
+  </si>
+  <si>
+    <t>ID-309</t>
+  </si>
+  <si>
     <t>Oregon</t>
   </si>
   <si>
     <t>Great horned owl</t>
   </si>
   <si>
+    <t>OR-360</t>
+  </si>
+  <si>
     <t>Common nighthawk</t>
   </si>
   <si>
+    <t>OR-170</t>
+  </si>
+  <si>
     <t>Western wood-pewee</t>
   </si>
   <si>
+    <t>OR-201</t>
+  </si>
+  <si>
+    <t>Hammond's flycatcher</t>
+  </si>
+  <si>
+    <t>OR-350</t>
+  </si>
+  <si>
     <t>Pacific-slope flycatcher</t>
   </si>
   <si>
+    <t>OR-362</t>
+  </si>
+  <si>
+    <t>Say's phoebe</t>
+  </si>
+  <si>
+    <t>OR-192</t>
+  </si>
+  <si>
+    <t>OR-331</t>
+  </si>
+  <si>
     <t>Tree swallow</t>
   </si>
   <si>
+    <t>OR-363</t>
+  </si>
+  <si>
     <t>Black-capped chickadee</t>
   </si>
   <si>
+    <t>OR-359</t>
+  </si>
+  <si>
     <t>Chickadees, titmouse</t>
   </si>
   <si>
@@ -334,324 +577,65 @@
     <t>Lazuli bunting</t>
   </si>
   <si>
+    <t>Swainson's thrush</t>
+  </si>
+  <si>
+    <t>OR-373</t>
+  </si>
+  <si>
+    <t>OR-324</t>
+  </si>
+  <si>
     <t>Orange-crowned warbler</t>
   </si>
   <si>
+    <t>OR-361</t>
+  </si>
+  <si>
+    <t>OR-295</t>
+  </si>
+  <si>
+    <t>OR-328</t>
+  </si>
+  <si>
+    <t>OR-354</t>
+  </si>
+  <si>
     <t>Fox sparrow</t>
   </si>
   <si>
+    <t>OR-345</t>
+  </si>
+  <si>
     <t>Song sparrow</t>
   </si>
   <si>
+    <t>OR-327</t>
+  </si>
+  <si>
     <t>Dark-eyed junco</t>
   </si>
   <si>
+    <t>OR-336</t>
+  </si>
+  <si>
     <t>Western tanager</t>
   </si>
   <si>
-    <t>VA-37</t>
-  </si>
-  <si>
-    <t>VA-55</t>
-  </si>
-  <si>
-    <t>VA-27</t>
-  </si>
-  <si>
-    <t>VA-85</t>
-  </si>
-  <si>
-    <t>VA-24</t>
-  </si>
-  <si>
-    <t>VA-53</t>
-  </si>
-  <si>
-    <t>VA-30</t>
-  </si>
-  <si>
-    <t>VA-73</t>
-  </si>
-  <si>
-    <t>VA-74</t>
-  </si>
-  <si>
-    <t>VA-22</t>
-  </si>
-  <si>
-    <t>VA-76</t>
-  </si>
-  <si>
-    <t>VA-43</t>
-  </si>
-  <si>
-    <t>VA-61</t>
-  </si>
-  <si>
-    <t>VA-52</t>
-  </si>
-  <si>
-    <t>VA-35</t>
-  </si>
-  <si>
-    <t>VA-39</t>
-  </si>
-  <si>
-    <t>VA-38</t>
-  </si>
-  <si>
-    <t>VA-26</t>
-  </si>
-  <si>
-    <t>KY-144</t>
-  </si>
-  <si>
-    <t>KY-82</t>
-  </si>
-  <si>
-    <t>KY-128</t>
-  </si>
-  <si>
-    <t>KY-72</t>
-  </si>
-  <si>
-    <t>KY-105</t>
-  </si>
-  <si>
-    <t>KY-75</t>
-  </si>
-  <si>
-    <t>KY-86</t>
-  </si>
-  <si>
-    <t>KY-120</t>
-  </si>
-  <si>
-    <t>IL-127</t>
-  </si>
-  <si>
-    <t>IL-126</t>
-  </si>
-  <si>
-    <t>IL-88</t>
-  </si>
-  <si>
-    <t>IL-130</t>
-  </si>
-  <si>
-    <t>IL-108</t>
-  </si>
-  <si>
-    <t>IL-146</t>
-  </si>
-  <si>
-    <t>MO-13</t>
-  </si>
-  <si>
-    <t>MO-129</t>
-  </si>
-  <si>
-    <t>MO-150</t>
-  </si>
-  <si>
-    <t>MO-151</t>
-  </si>
-  <si>
-    <t>MO-140</t>
-  </si>
-  <si>
-    <t>MO-145</t>
-  </si>
-  <si>
-    <t>KS-173</t>
-  </si>
-  <si>
-    <t>KS-175</t>
-  </si>
-  <si>
-    <t>KS-174</t>
-  </si>
-  <si>
-    <t>KS-176</t>
-  </si>
-  <si>
-    <t>KS-186</t>
-  </si>
-  <si>
-    <t>KS-177</t>
-  </si>
-  <si>
-    <t>CO-195</t>
-  </si>
-  <si>
-    <t>CO-284</t>
-  </si>
-  <si>
-    <t>CO-256</t>
-  </si>
-  <si>
-    <t>CO-194</t>
-  </si>
-  <si>
-    <t>CO-216</t>
-  </si>
-  <si>
-    <t>CO-213</t>
-  </si>
-  <si>
-    <t>CO-193</t>
-  </si>
-  <si>
-    <t>CO-280</t>
-  </si>
-  <si>
-    <t>CO-139</t>
-  </si>
-  <si>
-    <t>WY-261</t>
-  </si>
-  <si>
-    <t>WY-260</t>
-  </si>
-  <si>
-    <t>WY-69</t>
-  </si>
-  <si>
-    <t>WY-253</t>
-  </si>
-  <si>
-    <t>WY-264</t>
-  </si>
-  <si>
-    <t>MT-285</t>
-  </si>
-  <si>
-    <t>MT-277</t>
-  </si>
-  <si>
-    <t>MT-269</t>
-  </si>
-  <si>
-    <t>ID-202</t>
-  </si>
-  <si>
-    <t>ID-323</t>
-  </si>
-  <si>
-    <t>ID-302</t>
-  </si>
-  <si>
-    <t>ID-309</t>
-  </si>
-  <si>
-    <t>OR-360</t>
-  </si>
-  <si>
-    <t>OR-170</t>
-  </si>
-  <si>
-    <t>OR-201</t>
-  </si>
-  <si>
-    <t>OR-350</t>
-  </si>
-  <si>
-    <t>OR-362</t>
-  </si>
-  <si>
-    <t>OR-192</t>
-  </si>
-  <si>
-    <t>OR-331</t>
-  </si>
-  <si>
-    <t>OR-363</t>
-  </si>
-  <si>
-    <t>OR-359</t>
-  </si>
-  <si>
-    <t>OR-373</t>
-  </si>
-  <si>
-    <t>OR-324</t>
-  </si>
-  <si>
-    <t>OR-361</t>
-  </si>
-  <si>
-    <t>OR-295</t>
-  </si>
-  <si>
-    <t>OR-328</t>
-  </si>
-  <si>
-    <t>OR-354</t>
-  </si>
-  <si>
-    <t>OR-345</t>
-  </si>
-  <si>
-    <t>OR-327</t>
-  </si>
-  <si>
-    <t>OR-336</t>
-  </si>
-  <si>
     <t>OR-246</t>
   </si>
   <si>
     <t>OR-313</t>
-  </si>
-  <si>
-    <t>Chuck-will's-widow</t>
-  </si>
-  <si>
-    <t>Bell's vireo</t>
-  </si>
-  <si>
-    <t>Brewer's sparrow</t>
-  </si>
-  <si>
-    <t>Lincoln's sparrow</t>
-  </si>
-  <si>
-    <t>Cassin's finch</t>
-  </si>
-  <si>
-    <t>Hammond's flycatcher</t>
-  </si>
-  <si>
-    <t>Say's phoebe</t>
-  </si>
-  <si>
-    <t>Swainson's thrush</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -674,16 +658,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -691,15 +667,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1031,14 +999,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="4" max="4" width="28" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="120">
       <c r="A1" t="s">
@@ -1083,19 +1046,19 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1109,22 +1072,22 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H3">
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1138,22 +1101,22 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H4">
         <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1167,22 +1130,22 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1196,22 +1159,22 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H6">
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1225,22 +1188,22 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H7">
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1254,22 +1217,22 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H8">
         <v>12</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1283,22 +1246,22 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>32</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H9">
         <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1312,22 +1275,22 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H10">
         <v>13</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1341,22 +1304,22 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H11">
         <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1370,22 +1333,22 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="F12">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H12">
         <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1399,22 +1362,22 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H13">
         <v>13</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1428,22 +1391,22 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>43</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H14">
         <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1457,22 +1420,22 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="F15">
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H15">
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1486,22 +1449,22 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="F16">
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H16">
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1515,22 +1478,22 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="F17">
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H17">
         <v>14</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1544,22 +1507,22 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="F18">
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H18">
         <v>15</v>
       </c>
       <c r="J18" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1573,22 +1536,22 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>126</v>
+        <v>55</v>
       </c>
       <c r="F19">
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H19">
         <v>15</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1599,25 +1562,25 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H20">
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1628,25 +1591,25 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>128</v>
+        <v>60</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H21">
         <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1657,25 +1620,25 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>61</v>
       </c>
       <c r="F22">
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H22">
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1686,25 +1649,25 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="F23">
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H23">
         <v>11</v>
       </c>
       <c r="J23" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1715,25 +1678,25 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="F24">
         <v>5</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H24">
         <v>12</v>
       </c>
       <c r="J24" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1744,25 +1707,25 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>67</v>
       </c>
       <c r="F25">
         <v>6</v>
       </c>
       <c r="G25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H25">
         <v>13</v>
       </c>
       <c r="J25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1773,25 +1736,25 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="F26">
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H26">
         <v>13</v>
       </c>
       <c r="J26" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1802,25 +1765,25 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
-        <v>134</v>
+        <v>71</v>
       </c>
       <c r="F27">
         <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="H27">
         <v>17</v>
       </c>
       <c r="J27" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1831,25 +1794,25 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>135</v>
+        <v>76</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
       <c r="J28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1860,25 +1823,25 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="E29" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="H29">
         <v>7</v>
       </c>
       <c r="J29" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1889,25 +1852,25 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="F30">
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H30">
         <v>13</v>
       </c>
       <c r="J30" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1918,25 +1881,25 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
+        <v>83</v>
       </c>
       <c r="F31">
         <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H31">
         <v>15</v>
       </c>
       <c r="J31" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1947,25 +1910,25 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="E32" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="F32">
         <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H32">
         <v>15</v>
       </c>
       <c r="J32" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1976,25 +1939,25 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="E33" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="F33">
         <v>6</v>
       </c>
       <c r="G33" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="H33">
         <v>16</v>
       </c>
       <c r="J33" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2005,25 +1968,25 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="E34" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H34">
         <v>2</v>
       </c>
       <c r="J34" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2034,25 +1997,25 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="E35" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="F35">
         <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H35">
         <v>4</v>
       </c>
       <c r="J35" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2063,25 +2026,25 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="F36">
         <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H36">
         <v>4</v>
       </c>
       <c r="J36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2092,25 +2055,25 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>195</v>
+        <v>97</v>
       </c>
       <c r="E37" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="F37">
         <v>4</v>
       </c>
       <c r="G37" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="H37">
         <v>5</v>
       </c>
       <c r="J37" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2121,25 +2084,25 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="E38" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="F38">
         <v>5</v>
       </c>
       <c r="G38" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H38">
         <v>13</v>
       </c>
       <c r="J38" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2150,25 +2113,25 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="E39" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="F39">
         <v>6</v>
       </c>
       <c r="G39" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H39">
         <v>14</v>
       </c>
       <c r="J39" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2179,25 +2142,25 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H40">
         <v>4</v>
       </c>
       <c r="J40" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2208,25 +2171,25 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E41" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="F41">
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H41">
         <v>4</v>
       </c>
       <c r="J41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2237,25 +2200,25 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E42" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="F42">
         <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H42">
         <v>4</v>
       </c>
       <c r="J42" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2266,25 +2229,25 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="F43">
         <v>4</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H43">
         <v>4</v>
       </c>
       <c r="J43" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2295,25 +2258,25 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E44" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="F44">
         <v>5</v>
       </c>
       <c r="G44" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H44">
         <v>12</v>
       </c>
       <c r="J44" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2324,25 +2287,25 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="F45">
         <v>6</v>
       </c>
       <c r="G45" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="H45">
         <v>16</v>
       </c>
       <c r="J45" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2353,25 +2316,25 @@
         <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="E46" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H46">
         <v>4</v>
       </c>
       <c r="J46" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2382,25 +2345,25 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="E47" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="F47">
         <v>2</v>
       </c>
       <c r="G47" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="H47">
         <v>6</v>
       </c>
       <c r="J47" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2411,25 +2374,25 @@
         <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="E48" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="F48">
         <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H48">
         <v>11</v>
       </c>
       <c r="J48" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2440,25 +2403,25 @@
         <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="E49" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="F49">
         <v>4</v>
       </c>
       <c r="G49" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H49">
         <v>14</v>
       </c>
       <c r="J49" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2469,25 +2432,25 @@
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D50" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="E50" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="F50">
         <v>5</v>
       </c>
       <c r="G50" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H50">
         <v>14</v>
       </c>
       <c r="J50" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2498,25 +2461,25 @@
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
-        <v>197</v>
+        <v>127</v>
       </c>
       <c r="E51" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="F51">
         <v>6</v>
       </c>
       <c r="G51" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H51">
         <v>14</v>
       </c>
       <c r="J51" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2527,25 +2490,25 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D52" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="E52" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="F52">
         <v>7</v>
       </c>
       <c r="G52" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H52">
         <v>15</v>
       </c>
       <c r="J52" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2556,25 +2519,25 @@
         <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D53" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="E53" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="F53">
         <v>8</v>
       </c>
       <c r="G53" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="H53">
         <v>16</v>
       </c>
       <c r="J53" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2585,25 +2548,25 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D54" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="E54" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="F54">
         <v>9</v>
       </c>
       <c r="G54" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="H54">
         <v>18</v>
       </c>
       <c r="J54" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2614,25 +2577,25 @@
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="E55" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2643,25 +2606,25 @@
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="E56" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="F56">
         <v>2</v>
       </c>
       <c r="G56" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H56">
         <v>11</v>
       </c>
       <c r="J56" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2672,25 +2635,25 @@
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="E57" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="F57">
         <v>3</v>
       </c>
       <c r="G57" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H57">
         <v>13</v>
       </c>
       <c r="J57" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2701,25 +2664,25 @@
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="D58" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="E58" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="F58">
         <v>4</v>
       </c>
       <c r="G58" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H58">
         <v>14</v>
       </c>
       <c r="J58" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2730,25 +2693,25 @@
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="E59" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="F59">
         <v>5</v>
       </c>
       <c r="G59" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="H59">
         <v>17</v>
       </c>
       <c r="J59" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2759,25 +2722,25 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E60" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="F60">
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H60">
         <v>11</v>
       </c>
       <c r="J60" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2788,25 +2751,25 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="D61" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="E61" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="F61">
         <v>2</v>
       </c>
       <c r="G61" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H61">
         <v>12</v>
       </c>
       <c r="J61" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2817,25 +2780,25 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="E62" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="F62">
         <v>3</v>
       </c>
       <c r="G62" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H62">
         <v>14</v>
       </c>
       <c r="J62" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2846,25 +2809,25 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="D63" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="E63" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H63">
         <v>4</v>
       </c>
       <c r="J63" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2875,25 +2838,25 @@
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="D64" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="E64" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="F64">
         <v>2</v>
       </c>
       <c r="G64" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H64">
         <v>11</v>
       </c>
       <c r="J64" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2904,25 +2867,25 @@
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="D65" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="E65" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F65">
         <v>3</v>
       </c>
       <c r="G65" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H65">
         <v>13</v>
       </c>
       <c r="J65" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2933,25 +2896,25 @@
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="D66" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="E66" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F66">
         <v>4</v>
       </c>
       <c r="G66" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H66">
         <v>13</v>
       </c>
       <c r="J66" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2962,25 +2925,25 @@
         <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D67" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="E67" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F67">
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H67">
         <v>2</v>
       </c>
       <c r="J67" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2991,25 +2954,25 @@
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D68" t="s">
-        <v>94</v>
+        <v>165</v>
       </c>
       <c r="E68" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F68">
         <v>2</v>
       </c>
       <c r="G68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H68">
         <v>3</v>
       </c>
       <c r="J68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -3020,25 +2983,25 @@
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D69" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
       <c r="E69" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F69">
         <v>3</v>
       </c>
       <c r="G69" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H69">
         <v>4</v>
       </c>
       <c r="J69" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3049,25 +3012,25 @@
         <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D70" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="E70" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F70">
         <v>4</v>
       </c>
       <c r="G70" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H70">
         <v>4</v>
       </c>
       <c r="J70" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -3078,25 +3041,25 @@
         <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D71" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="E71" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F71">
         <v>5</v>
       </c>
       <c r="G71" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H71">
         <v>4</v>
       </c>
       <c r="J71" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -3107,25 +3070,25 @@
         <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D72" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="E72" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F72">
         <v>6</v>
       </c>
       <c r="G72" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H72">
         <v>4</v>
       </c>
       <c r="J72" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -3136,25 +3099,25 @@
         <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D73" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E73" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F73">
         <v>7</v>
       </c>
       <c r="G73" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H73">
         <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -3165,25 +3128,25 @@
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D74" t="s">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="E74" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F74">
         <v>8</v>
       </c>
       <c r="G74" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="H74">
         <v>7</v>
       </c>
       <c r="J74" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -3194,25 +3157,25 @@
         <v>10</v>
       </c>
       <c r="C75" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D75" t="s">
-        <v>98</v>
+        <v>178</v>
       </c>
       <c r="E75" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F75">
         <v>9</v>
       </c>
       <c r="G75" t="s">
-        <v>99</v>
+        <v>180</v>
       </c>
       <c r="H75">
         <v>15</v>
       </c>
       <c r="J75" t="s">
-        <v>99</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -3223,25 +3186,25 @@
         <v>10</v>
       </c>
       <c r="C76" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D76" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="E76" t="s">
-        <v>101</v>
+        <v>182</v>
       </c>
       <c r="F76">
         <v>10</v>
       </c>
       <c r="G76" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
       <c r="H76">
         <v>9</v>
       </c>
       <c r="J76" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -3252,25 +3215,25 @@
         <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D77" t="s">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="E77" t="s">
-        <v>101</v>
+        <v>182</v>
       </c>
       <c r="F77">
         <v>11</v>
       </c>
       <c r="G77" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H77">
         <v>15</v>
       </c>
       <c r="J77" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -3281,25 +3244,25 @@
         <v>10</v>
       </c>
       <c r="C78" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D78" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="E78" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F78">
         <v>12</v>
       </c>
       <c r="G78" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H78">
         <v>11</v>
       </c>
       <c r="J78" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -3310,25 +3273,25 @@
         <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D79" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="E79" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F79">
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H79">
         <v>12</v>
       </c>
       <c r="J79" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -3339,25 +3302,25 @@
         <v>10</v>
       </c>
       <c r="C80" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D80" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="E80" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F80">
         <v>14</v>
       </c>
       <c r="G80" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H80">
         <v>13</v>
       </c>
       <c r="J80" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3368,25 +3331,25 @@
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D81" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E81" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F81">
         <v>15</v>
       </c>
       <c r="G81" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H81">
         <v>13</v>
       </c>
       <c r="J81" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3397,25 +3360,25 @@
         <v>10</v>
       </c>
       <c r="C82" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D82" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E82" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F82">
         <v>16</v>
       </c>
       <c r="G82" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H82">
         <v>13</v>
       </c>
       <c r="J82" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3426,25 +3389,25 @@
         <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D83" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="E83" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F83">
         <v>17</v>
       </c>
       <c r="G83" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H83">
         <v>14</v>
       </c>
       <c r="J83" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3455,25 +3418,25 @@
         <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D84" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="E84" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F84">
         <v>18</v>
       </c>
       <c r="G84" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H84">
         <v>11</v>
       </c>
       <c r="J84" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3484,25 +3447,25 @@
         <v>10</v>
       </c>
       <c r="C85" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D85" t="s">
-        <v>105</v>
+        <v>193</v>
       </c>
       <c r="E85" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F85">
         <v>19</v>
       </c>
       <c r="G85" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H85">
         <v>14</v>
       </c>
       <c r="J85" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3513,25 +3476,25 @@
         <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D86" t="s">
-        <v>106</v>
+        <v>195</v>
       </c>
       <c r="E86" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F86">
         <v>20</v>
       </c>
       <c r="G86" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H86">
         <v>14</v>
       </c>
       <c r="J86" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -3542,25 +3505,25 @@
         <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D87" t="s">
-        <v>107</v>
+        <v>197</v>
       </c>
       <c r="E87" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="F87">
         <v>21</v>
       </c>
       <c r="G87" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H87">
         <v>14</v>
       </c>
       <c r="J87" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3571,25 +3534,25 @@
         <v>10</v>
       </c>
       <c r="C88" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D88" t="s">
-        <v>108</v>
+        <v>199</v>
       </c>
       <c r="E88" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="F88">
         <v>22</v>
       </c>
       <c r="G88" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H88">
         <v>15</v>
       </c>
       <c r="J88" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3600,30 +3563,29 @@
         <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="D89" t="s">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="E89" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="F89">
         <v>23</v>
       </c>
       <c r="G89" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="H89">
         <v>15</v>
       </c>
       <c r="J89" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>